<commit_message>
Updated TT and state type
</commit_message>
<xml_diff>
--- a/Ax2/Transition_Table.xlsx
+++ b/Ax2/Transition_Table.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e013e576aa07c75d/Documents/GitHub/Flowcode/Ax2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\25W\CST8152 Complier\git clone\Flowcode\Ax2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{1BC781FB-0E67-4881-B884-083F46ED3881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67BB7957-25E0-4CD6-867C-A024DD27FF6B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A61214-8B6E-4785-9D10-83065B5482EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{D4CAA7EB-27A3-41A0-A611-5E33AE82081F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{D4CAA7EB-27A3-41A0-A611-5E33AE82081F}"/>
   </bookViews>
   <sheets>
     <sheet name="VERSION1" sheetId="1" r:id="rId1"/>
     <sheet name="VERSION2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="FINAL(HOPEFULLY...)" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1240" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="98">
   <si>
     <t>L (a-zA-Z)</t>
   </si>
@@ -417,12 +418,60 @@
   <si>
     <t>FSNR(COMMENT END)</t>
   </si>
+  <si>
+    <t>FSWR(ID)</t>
+  </si>
+  <si>
+    <t>FSWR(INTEGER)</t>
+  </si>
+  <si>
+    <t>ESWR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ESNR</t>
+  </si>
+  <si>
+    <t>FSWR(KEY)</t>
+  </si>
+  <si>
+    <t>FSWR(DOUBLE)</t>
+  </si>
+  <si>
+    <t>FSNR(STRING )</t>
+  </si>
+  <si>
+    <t>FSWR(MULTIPLY)</t>
+  </si>
+  <si>
+    <t>FSNR(GREATER THAN EQUAL)</t>
+  </si>
+  <si>
+    <t>FSWR(GREATER)</t>
+  </si>
+  <si>
+    <t>FSNR(LESS THAN EQUAL)</t>
+  </si>
+  <si>
+    <t>FSWR(LESS)</t>
+  </si>
+  <si>
+    <t>FSNR(EQUAL)</t>
+  </si>
+  <si>
+    <t>FSWR(ASSIGNMENT)</t>
+  </si>
+  <si>
+    <t>FSNR(NOT)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,6 +505,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -483,7 +538,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -506,11 +561,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -540,6 +610,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -881,12 +961,12 @@
       <selection pane="bottomLeft" activeCell="F1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="35.450000000000003" customHeight="1" thickBot="1">
+    <row r="1" spans="1:27" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -967,7 +1047,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="43.5" thickBot="1">
+    <row r="2" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -1050,7 +1130,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="57.75" thickBot="1">
+    <row r="3" spans="1:27" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1131,7 +1211,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="48" thickBot="1">
+    <row r="4" spans="1:27" ht="49.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1212,7 +1292,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="66.75" thickBot="1">
+    <row r="5" spans="1:27" ht="70.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1293,7 +1373,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="43.5" thickBot="1">
+    <row r="6" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1374,7 +1454,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="43.5" thickBot="1">
+    <row r="7" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1455,7 +1535,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15.75" thickBot="1">
+    <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1536,7 +1616,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="57.75" thickBot="1">
+    <row r="9" spans="1:27" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1617,7 +1697,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="86.25" thickBot="1">
+    <row r="10" spans="1:27" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1700,7 +1780,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="57.75" thickBot="1">
+    <row r="11" spans="1:27" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1783,7 +1863,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="86.25" thickBot="1">
+    <row r="12" spans="1:27" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1866,7 +1946,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="57.75" thickBot="1">
+    <row r="13" spans="1:27" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1949,7 +2029,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="29.25" thickBot="1">
+    <row r="14" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -2032,7 +2112,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="86.25" thickBot="1">
+    <row r="15" spans="1:27" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2115,7 +2195,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="57.75" thickBot="1">
+    <row r="16" spans="1:27" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -2198,7 +2278,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="43.5" thickBot="1">
+    <row r="17" spans="1:27" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2281,7 +2361,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="72" thickBot="1">
+    <row r="18" spans="1:27" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -2364,7 +2444,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="57.75" thickBot="1">
+    <row r="19" spans="1:27" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2447,7 +2527,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="86.25" thickBot="1">
+    <row r="20" spans="1:27" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -2530,7 +2610,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="43.5" thickBot="1">
+    <row r="21" spans="1:27" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -2622,22 +2702,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1317344A-6E95-45DA-A395-13D4B567695A}">
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P1" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="9"/>
-    <col min="3" max="3" width="8.85546875" style="9" customWidth="1"/>
-    <col min="4" max="26" width="8.85546875" style="9"/>
+    <col min="1" max="1" width="3.88671875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="9"/>
+    <col min="3" max="3" width="8.88671875" style="9" customWidth="1"/>
+    <col min="4" max="26" width="8.88671875" style="9"/>
     <col min="27" max="27" width="25" style="9" customWidth="1"/>
-    <col min="28" max="16384" width="8.85546875" style="9"/>
+    <col min="28" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="35.450000000000003" customHeight="1" thickBot="1">
+    <row r="1" spans="1:27" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6"/>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -2718,7 +2798,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="15.75" thickBot="1">
+    <row r="2" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>0</v>
       </c>
@@ -2801,7 +2881,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.75" thickBot="1">
+    <row r="3" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -2884,7 +2964,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15.75" thickBot="1">
+    <row r="4" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -2967,7 +3047,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15.75" thickBot="1">
+    <row r="5" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -3050,7 +3130,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15.75" thickBot="1">
+    <row r="6" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -3133,7 +3213,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15.75" thickBot="1">
+    <row r="7" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -3216,7 +3296,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15.75" thickBot="1">
+    <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -3299,7 +3379,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15.75" thickBot="1">
+    <row r="9" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -3382,7 +3462,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15.75" thickBot="1">
+    <row r="10" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -3465,7 +3545,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.75" thickBot="1">
+    <row r="11" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -3548,7 +3628,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15.75" thickBot="1">
+    <row r="12" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -3631,7 +3711,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15.75" thickBot="1">
+    <row r="13" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -3714,7 +3794,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.75" thickBot="1">
+    <row r="14" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -3797,7 +3877,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15.75" thickBot="1">
+    <row r="15" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -3880,7 +3960,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="15.75" thickBot="1">
+    <row r="16" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8">
         <v>14</v>
       </c>
@@ -3963,7 +4043,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15.75" thickBot="1">
+    <row r="17" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8">
         <v>15</v>
       </c>
@@ -4046,7 +4126,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="15.75" thickBot="1">
+    <row r="18" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8">
         <v>16</v>
       </c>
@@ -4129,7 +4209,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="15.75" thickBot="1">
+    <row r="19" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8">
         <v>17</v>
       </c>
@@ -4212,7 +4292,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="15.75" thickBot="1">
+    <row r="20" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8">
         <v>18</v>
       </c>
@@ -4295,7 +4375,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="15.75" thickBot="1">
+    <row r="21" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8">
         <v>19</v>
       </c>
@@ -4378,7 +4458,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="15.75" thickBot="1">
+    <row r="22" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8">
         <v>20</v>
       </c>
@@ -4461,7 +4541,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="15.75" thickBot="1">
+    <row r="23" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8">
         <v>21</v>
       </c>
@@ -4544,7 +4624,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="15.75" thickBot="1">
+    <row r="24" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8">
         <v>22</v>
       </c>
@@ -4627,7 +4707,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="15.75" thickBot="1">
+    <row r="25" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8">
         <v>23</v>
       </c>
@@ -4719,31 +4799,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5BBC166-234D-46C0-97DE-1E02EB766277}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="9"/>
+    <col min="2" max="2" width="10.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="35.450000000000003" customHeight="1" thickBot="1">
+    <row r="1" spans="1:15" ht="35.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6"/>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -4788,7 +4869,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1">
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>0</v>
       </c>
@@ -4796,7 +4877,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" s="8">
         <v>1</v>
@@ -4835,101 +4916,101 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1">
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>26</v>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2</v>
       </c>
       <c r="G3" s="8">
         <v>2</v>
       </c>
       <c r="H3" s="8">
-        <v>5</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="I3" s="8">
+        <v>2</v>
+      </c>
+      <c r="J3" s="8">
+        <v>2</v>
+      </c>
+      <c r="K3" s="8">
+        <v>2</v>
+      </c>
+      <c r="L3" s="11">
+        <v>2</v>
+      </c>
+      <c r="M3" s="8">
+        <v>2</v>
+      </c>
+      <c r="N3" s="8">
+        <v>2</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="8">
-        <v>3</v>
+        <v>39</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -4976,7 +5057,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1">
+    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -5023,7 +5104,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1">
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -5070,7 +5151,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1">
+    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -5117,7 +5198,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1">
+    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -5164,7 +5245,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1">
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -5211,7 +5292,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1">
+    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -5258,7 +5339,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1">
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -5305,7 +5386,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" thickBot="1">
+    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -5352,7 +5433,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1">
+    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -5399,7 +5480,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1">
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -5446,7 +5527,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1">
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8">
         <v>14</v>
       </c>
@@ -5493,7 +5574,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" thickBot="1">
+    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8">
         <v>15</v>
       </c>
@@ -5540,7 +5621,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1">
+    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8">
         <v>16</v>
       </c>
@@ -5587,7 +5668,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" thickBot="1">
+    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="8">
         <v>17</v>
       </c>
@@ -5634,7 +5715,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15.75" thickBot="1">
+    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="8">
         <v>18</v>
       </c>
@@ -5681,7 +5762,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15.75" thickBot="1">
+    <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="8">
         <v>19</v>
       </c>
@@ -5728,7 +5809,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15.75" thickBot="1">
+    <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="8">
         <v>20</v>
       </c>
@@ -5775,7 +5856,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15.75" thickBot="1">
+    <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="8">
         <v>21</v>
       </c>
@@ -5822,7 +5903,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15.75" thickBot="1">
+    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="8">
         <v>22</v>
       </c>
@@ -5869,7 +5950,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15.75" thickBot="1">
+    <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8">
         <v>23</v>
       </c>
@@ -5914,6 +5995,1387 @@
       </c>
       <c r="O25" s="8" t="s">
         <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D7EB35-C198-4C0D-A3DA-50BE50F84B53}">
+  <dimension ref="A1:O29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="15" max="15" width="24.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="12"/>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
+        <v>0</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14">
+        <v>1</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="K2" s="14">
+        <v>10</v>
+      </c>
+      <c r="L2" s="14">
+        <v>12</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14">
+        <v>3</v>
+      </c>
+      <c r="D3" s="14">
+        <v>3</v>
+      </c>
+      <c r="E3" s="14">
+        <v>2</v>
+      </c>
+      <c r="F3" s="14">
+        <v>2</v>
+      </c>
+      <c r="G3" s="14">
+        <v>2</v>
+      </c>
+      <c r="H3" s="14">
+        <v>2</v>
+      </c>
+      <c r="I3" s="14">
+        <v>2</v>
+      </c>
+      <c r="J3" s="14">
+        <v>2</v>
+      </c>
+      <c r="K3" s="14">
+        <v>2</v>
+      </c>
+      <c r="L3" s="14">
+        <v>2</v>
+      </c>
+      <c r="M3" s="14">
+        <v>2</v>
+      </c>
+      <c r="N3" s="14">
+        <v>2</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="14">
+        <v>2</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="14">
+        <v>3</v>
+      </c>
+      <c r="B5" s="14">
+        <v>3</v>
+      </c>
+      <c r="C5" s="14">
+        <v>3</v>
+      </c>
+      <c r="D5" s="14">
+        <v>3</v>
+      </c>
+      <c r="E5" s="14">
+        <v>4</v>
+      </c>
+      <c r="F5" s="14">
+        <v>4</v>
+      </c>
+      <c r="G5" s="14">
+        <v>4</v>
+      </c>
+      <c r="H5" s="14">
+        <v>4</v>
+      </c>
+      <c r="I5" s="14">
+        <v>4</v>
+      </c>
+      <c r="J5" s="14">
+        <v>4</v>
+      </c>
+      <c r="K5" s="14">
+        <v>4</v>
+      </c>
+      <c r="L5" s="14">
+        <v>4</v>
+      </c>
+      <c r="M5" s="14">
+        <v>4</v>
+      </c>
+      <c r="N5" s="14">
+        <v>4</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="14">
+        <v>4</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
+        <v>5</v>
+      </c>
+      <c r="B7" s="14">
+        <v>6</v>
+      </c>
+      <c r="C7" s="14">
+        <v>5</v>
+      </c>
+      <c r="D7" s="14">
+        <v>6</v>
+      </c>
+      <c r="E7" s="14">
+        <v>7</v>
+      </c>
+      <c r="F7" s="14">
+        <v>6</v>
+      </c>
+      <c r="G7" s="14">
+        <v>6</v>
+      </c>
+      <c r="H7" s="14">
+        <v>6</v>
+      </c>
+      <c r="I7" s="14">
+        <v>6</v>
+      </c>
+      <c r="J7" s="14">
+        <v>6</v>
+      </c>
+      <c r="K7" s="14">
+        <v>6</v>
+      </c>
+      <c r="L7" s="14">
+        <v>6</v>
+      </c>
+      <c r="M7" s="14">
+        <v>6</v>
+      </c>
+      <c r="N7" s="14">
+        <v>6</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>6</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>7</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="14">
+        <v>8</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="14">
+        <v>8</v>
+      </c>
+      <c r="B10" s="14">
+        <v>9</v>
+      </c>
+      <c r="C10" s="14">
+        <v>8</v>
+      </c>
+      <c r="D10" s="14">
+        <v>9</v>
+      </c>
+      <c r="E10" s="14">
+        <v>9</v>
+      </c>
+      <c r="F10" s="14">
+        <v>9</v>
+      </c>
+      <c r="G10" s="14">
+        <v>9</v>
+      </c>
+      <c r="H10" s="14">
+        <v>9</v>
+      </c>
+      <c r="I10" s="14">
+        <v>9</v>
+      </c>
+      <c r="J10" s="14">
+        <v>9</v>
+      </c>
+      <c r="K10" s="14">
+        <v>9</v>
+      </c>
+      <c r="L10" s="14">
+        <v>9</v>
+      </c>
+      <c r="M10" s="14">
+        <v>9</v>
+      </c>
+      <c r="N10" s="14">
+        <v>9</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
+        <v>9</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
+        <v>10</v>
+      </c>
+      <c r="B12" s="14">
+        <v>10</v>
+      </c>
+      <c r="C12" s="14">
+        <v>10</v>
+      </c>
+      <c r="D12" s="14">
+        <v>10</v>
+      </c>
+      <c r="E12" s="14">
+        <v>10</v>
+      </c>
+      <c r="F12" s="14">
+        <v>10</v>
+      </c>
+      <c r="G12" s="14">
+        <v>10</v>
+      </c>
+      <c r="H12" s="14">
+        <v>10</v>
+      </c>
+      <c r="I12" s="14">
+        <v>10</v>
+      </c>
+      <c r="J12" s="14">
+        <v>10</v>
+      </c>
+      <c r="K12" s="14">
+        <v>11</v>
+      </c>
+      <c r="L12" s="14">
+        <v>10</v>
+      </c>
+      <c r="M12" s="14">
+        <v>10</v>
+      </c>
+      <c r="N12" s="14">
+        <v>10</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>11</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O13" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="14">
+        <v>12</v>
+      </c>
+      <c r="C14" s="14">
+        <v>12</v>
+      </c>
+      <c r="D14" s="14">
+        <v>12</v>
+      </c>
+      <c r="E14" s="14">
+        <v>12</v>
+      </c>
+      <c r="F14" s="14">
+        <v>12</v>
+      </c>
+      <c r="G14" s="14">
+        <v>12</v>
+      </c>
+      <c r="H14" s="14">
+        <v>12</v>
+      </c>
+      <c r="I14" s="14">
+        <v>12</v>
+      </c>
+      <c r="J14" s="14">
+        <v>12</v>
+      </c>
+      <c r="K14" s="14">
+        <v>12</v>
+      </c>
+      <c r="L14" s="14">
+        <v>13</v>
+      </c>
+      <c r="M14" s="14">
+        <v>12</v>
+      </c>
+      <c r="N14" s="14">
+        <v>12</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>13</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
+        <v>14</v>
+      </c>
+      <c r="B16" s="14">
+        <v>15</v>
+      </c>
+      <c r="C16" s="14">
+        <v>15</v>
+      </c>
+      <c r="D16" s="14">
+        <v>15</v>
+      </c>
+      <c r="E16" s="14">
+        <v>15</v>
+      </c>
+      <c r="F16" s="14">
+        <v>16</v>
+      </c>
+      <c r="G16" s="14">
+        <v>15</v>
+      </c>
+      <c r="H16" s="14">
+        <v>15</v>
+      </c>
+      <c r="I16" s="14">
+        <v>15</v>
+      </c>
+      <c r="J16" s="14">
+        <v>15</v>
+      </c>
+      <c r="K16" s="14">
+        <v>15</v>
+      </c>
+      <c r="L16" s="14">
+        <v>15</v>
+      </c>
+      <c r="M16" s="14">
+        <v>15</v>
+      </c>
+      <c r="N16" s="14">
+        <v>15</v>
+      </c>
+      <c r="O16" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
+        <v>15</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O17" s="14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="14">
+        <v>16</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
+        <v>17</v>
+      </c>
+      <c r="B19" s="14">
+        <v>19</v>
+      </c>
+      <c r="C19" s="14">
+        <v>19</v>
+      </c>
+      <c r="D19" s="14">
+        <v>19</v>
+      </c>
+      <c r="E19" s="14">
+        <v>19</v>
+      </c>
+      <c r="F19" s="14">
+        <v>19</v>
+      </c>
+      <c r="G19" s="14">
+        <v>18</v>
+      </c>
+      <c r="H19" s="14">
+        <v>19</v>
+      </c>
+      <c r="I19" s="14">
+        <v>19</v>
+      </c>
+      <c r="J19" s="14">
+        <v>19</v>
+      </c>
+      <c r="K19" s="14">
+        <v>19</v>
+      </c>
+      <c r="L19" s="14">
+        <v>19</v>
+      </c>
+      <c r="M19" s="14">
+        <v>19</v>
+      </c>
+      <c r="N19" s="14">
+        <v>19</v>
+      </c>
+      <c r="O19" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="14">
+        <v>18</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O20" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
+        <v>19</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O21" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="14">
+        <v>20</v>
+      </c>
+      <c r="B22" s="14">
+        <v>22</v>
+      </c>
+      <c r="C22" s="14">
+        <v>22</v>
+      </c>
+      <c r="D22" s="14">
+        <v>22</v>
+      </c>
+      <c r="E22" s="14">
+        <v>22</v>
+      </c>
+      <c r="F22" s="14">
+        <v>22</v>
+      </c>
+      <c r="G22" s="14">
+        <v>21</v>
+      </c>
+      <c r="H22" s="14">
+        <v>22</v>
+      </c>
+      <c r="I22" s="14">
+        <v>22</v>
+      </c>
+      <c r="J22" s="14">
+        <v>22</v>
+      </c>
+      <c r="K22" s="14">
+        <v>22</v>
+      </c>
+      <c r="L22" s="14">
+        <v>22</v>
+      </c>
+      <c r="M22" s="14">
+        <v>22</v>
+      </c>
+      <c r="N22" s="14">
+        <v>22</v>
+      </c>
+      <c r="O22" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="14">
+        <v>21</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N23" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="14">
+        <v>22</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N24" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O24" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="14">
+        <v>23</v>
+      </c>
+      <c r="B25" s="14">
+        <v>25</v>
+      </c>
+      <c r="C25" s="14">
+        <v>25</v>
+      </c>
+      <c r="D25" s="14">
+        <v>25</v>
+      </c>
+      <c r="E25" s="14">
+        <v>25</v>
+      </c>
+      <c r="F25" s="14">
+        <v>25</v>
+      </c>
+      <c r="G25" s="14">
+        <v>24</v>
+      </c>
+      <c r="H25" s="14">
+        <v>25</v>
+      </c>
+      <c r="I25" s="14">
+        <v>25</v>
+      </c>
+      <c r="J25" s="14">
+        <v>25</v>
+      </c>
+      <c r="K25" s="14">
+        <v>25</v>
+      </c>
+      <c r="L25" s="14">
+        <v>25</v>
+      </c>
+      <c r="M25" s="14">
+        <v>25</v>
+      </c>
+      <c r="N25" s="14">
+        <v>25</v>
+      </c>
+      <c r="O25" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="14">
+        <v>24</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O26" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="14">
+        <v>25</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N27" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O27" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="14">
+        <v>26</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" s="14">
+        <v>27</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="M28" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="N28" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="O28" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="14">
+        <v>27</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="N29" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="O29" s="14" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>